<commit_message>
Final version for deployment
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af75e55b634f35c0/desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{7D5E251A-980C-4970-8124-C19BAC605134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CBF6E5E-20AA-4BCF-B9A8-AAFAB3BB802A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71288622-89B1-4B15-B1D1-C6CEC7466DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -582,10 +582,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,8 +618,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548F3BD-78D7-4C41-AEEB-86055749FC7F}">
   <dimension ref="A1:C325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,7 +981,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2">
@@ -984,7 +992,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">

</xml_diff>

<commit_message>
pill added dropdown removed
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71288622-89B1-4B15-B1D1-C6CEC7466DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4D21A9-0A6D-4558-BE6D-6D7C92FD6671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>CJ80E6FI</t>
   </si>
@@ -625,7 +625,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -955,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548F3BD-78D7-4C41-AEEB-86055749FC7F}">
-  <dimension ref="A1:C325"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +995,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>15</v>
       </c>
     </row>
@@ -995,7 +1006,7 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1003,10 +1014,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>25</v>
       </c>
     </row>
@@ -2610,10 +2621,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C150">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -2621,10 +2632,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C151">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -2632,10 +2643,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C152">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -2643,10 +2654,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C153">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -2654,10 +2665,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C154">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -2665,10 +2676,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C155">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -2676,10 +2687,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C156">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -2687,10 +2698,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C157">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -2698,10 +2709,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C158">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -2709,10 +2720,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C159">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -2720,10 +2731,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C160">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -2731,10 +2742,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C161">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -2742,10 +2753,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C162">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -2753,10 +2764,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C163">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -2764,10 +2775,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C164">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -2775,10 +2786,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C165">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -2786,10 +2797,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C166">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -2797,10 +2808,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C167">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -2808,10 +2819,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C168">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -2819,10 +2830,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C169">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -2830,10 +2841,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C170">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
@@ -2841,10 +2852,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C171">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
@@ -2852,10 +2863,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C172">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
@@ -2863,10 +2874,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C173">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
@@ -2874,10 +2885,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C174">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
@@ -2885,10 +2896,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C175">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
@@ -2896,10 +2907,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C176">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
@@ -2907,10 +2918,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C177">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
@@ -2918,1630 +2929,17 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C178">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179">
-        <v>178</v>
-      </c>
-      <c r="B179" t="s">
-        <v>176</v>
-      </c>
-      <c r="C179">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180">
-        <v>179</v>
-      </c>
-      <c r="B180" t="s">
-        <v>148</v>
-      </c>
-      <c r="C180">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181">
-        <v>180</v>
-      </c>
-      <c r="B181" t="s">
-        <v>149</v>
-      </c>
-      <c r="C181">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182">
-        <v>181</v>
-      </c>
-      <c r="B182" t="s">
-        <v>150</v>
-      </c>
-      <c r="C182">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183">
-        <v>182</v>
-      </c>
-      <c r="B183" t="s">
-        <v>151</v>
-      </c>
-      <c r="C183">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184">
-        <v>183</v>
-      </c>
-      <c r="B184" t="s">
-        <v>161</v>
-      </c>
-      <c r="C184">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185">
-        <v>184</v>
-      </c>
-      <c r="B185" t="s">
-        <v>162</v>
-      </c>
-      <c r="C185">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186">
-        <v>185</v>
-      </c>
-      <c r="B186" t="s">
-        <v>163</v>
-      </c>
-      <c r="C186">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187">
-        <v>186</v>
-      </c>
-      <c r="B187" t="s">
-        <v>164</v>
-      </c>
-      <c r="C187">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188">
-        <v>187</v>
-      </c>
-      <c r="B188" t="s">
-        <v>165</v>
-      </c>
-      <c r="C188">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189">
-        <v>188</v>
-      </c>
-      <c r="B189" t="s">
-        <v>166</v>
-      </c>
-      <c r="C189">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A190">
-        <v>189</v>
-      </c>
-      <c r="B190" t="s">
-        <v>167</v>
-      </c>
-      <c r="C190">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191">
-        <v>190</v>
-      </c>
-      <c r="B191" t="s">
-        <v>168</v>
-      </c>
-      <c r="C191">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192">
-        <v>191</v>
-      </c>
-      <c r="B192" t="s">
-        <v>169</v>
-      </c>
-      <c r="C192">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193">
-        <v>192</v>
-      </c>
-      <c r="B193" t="s">
-        <v>170</v>
-      </c>
-      <c r="C193">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A194">
-        <v>193</v>
-      </c>
-      <c r="B194" t="s">
-        <v>171</v>
-      </c>
-      <c r="C194">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195">
-        <v>194</v>
-      </c>
-      <c r="B195" t="s">
-        <v>172</v>
-      </c>
-      <c r="C195">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196">
-        <v>195</v>
-      </c>
-      <c r="B196" t="s">
-        <v>173</v>
-      </c>
-      <c r="C196">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197">
-        <v>196</v>
-      </c>
-      <c r="B197" t="s">
-        <v>174</v>
-      </c>
-      <c r="C197">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A198">
-        <v>197</v>
-      </c>
-      <c r="B198" t="s">
-        <v>175</v>
-      </c>
-      <c r="C198">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A199">
-        <v>198</v>
-      </c>
-      <c r="B199" t="s">
-        <v>176</v>
-      </c>
-      <c r="C199">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A200">
-        <v>199</v>
-      </c>
-      <c r="B200" t="s">
-        <v>148</v>
-      </c>
-      <c r="C200">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A201">
-        <v>200</v>
-      </c>
-      <c r="B201" t="s">
-        <v>149</v>
-      </c>
-      <c r="C201">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A202">
-        <v>201</v>
-      </c>
-      <c r="B202" t="s">
-        <v>150</v>
-      </c>
-      <c r="C202">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A203">
-        <v>202</v>
-      </c>
-      <c r="B203" t="s">
-        <v>151</v>
-      </c>
-      <c r="C203">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A204">
-        <v>203</v>
-      </c>
-      <c r="B204" t="s">
-        <v>161</v>
-      </c>
-      <c r="C204">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A205">
-        <v>204</v>
-      </c>
-      <c r="B205" t="s">
-        <v>162</v>
-      </c>
-      <c r="C205">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A206">
-        <v>205</v>
-      </c>
-      <c r="B206" t="s">
-        <v>163</v>
-      </c>
-      <c r="C206">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A207">
-        <v>206</v>
-      </c>
-      <c r="B207" t="s">
-        <v>164</v>
-      </c>
-      <c r="C207">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A208">
-        <v>207</v>
-      </c>
-      <c r="B208" t="s">
-        <v>165</v>
-      </c>
-      <c r="C208">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A209">
-        <v>208</v>
-      </c>
-      <c r="B209" t="s">
-        <v>166</v>
-      </c>
-      <c r="C209">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A210">
-        <v>209</v>
-      </c>
-      <c r="B210" t="s">
-        <v>167</v>
-      </c>
-      <c r="C210">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A211">
-        <v>210</v>
-      </c>
-      <c r="B211" t="s">
-        <v>168</v>
-      </c>
-      <c r="C211">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A212">
-        <v>211</v>
-      </c>
-      <c r="B212" t="s">
-        <v>169</v>
-      </c>
-      <c r="C212">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A213">
-        <v>212</v>
-      </c>
-      <c r="B213" t="s">
-        <v>170</v>
-      </c>
-      <c r="C213">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A214">
-        <v>213</v>
-      </c>
-      <c r="B214" t="s">
-        <v>171</v>
-      </c>
-      <c r="C214">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A215">
-        <v>214</v>
-      </c>
-      <c r="B215" t="s">
-        <v>172</v>
-      </c>
-      <c r="C215">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A216">
-        <v>215</v>
-      </c>
-      <c r="B216" t="s">
-        <v>173</v>
-      </c>
-      <c r="C216">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A217">
-        <v>216</v>
-      </c>
-      <c r="B217" t="s">
-        <v>174</v>
-      </c>
-      <c r="C217">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A218">
-        <v>217</v>
-      </c>
-      <c r="B218" t="s">
-        <v>175</v>
-      </c>
-      <c r="C218">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A219">
-        <v>218</v>
-      </c>
-      <c r="B219" t="s">
-        <v>176</v>
-      </c>
-      <c r="C219">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A220">
-        <v>219</v>
-      </c>
-      <c r="B220" t="s">
-        <v>148</v>
-      </c>
-      <c r="C220">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A221">
-        <v>220</v>
-      </c>
-      <c r="B221" t="s">
-        <v>149</v>
-      </c>
-      <c r="C221">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A222">
-        <v>221</v>
-      </c>
-      <c r="B222" t="s">
-        <v>150</v>
-      </c>
-      <c r="C222">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A223">
-        <v>222</v>
-      </c>
-      <c r="B223" t="s">
-        <v>151</v>
-      </c>
-      <c r="C223">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A224">
-        <v>223</v>
-      </c>
-      <c r="B224" t="s">
-        <v>161</v>
-      </c>
-      <c r="C224">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A225">
-        <v>224</v>
-      </c>
-      <c r="B225" t="s">
-        <v>162</v>
-      </c>
-      <c r="C225">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A226">
-        <v>225</v>
-      </c>
-      <c r="B226" t="s">
-        <v>163</v>
-      </c>
-      <c r="C226">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A227">
-        <v>226</v>
-      </c>
-      <c r="B227" t="s">
-        <v>164</v>
-      </c>
-      <c r="C227">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A228">
-        <v>227</v>
-      </c>
-      <c r="B228" t="s">
-        <v>165</v>
-      </c>
-      <c r="C228">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A229">
-        <v>228</v>
-      </c>
-      <c r="B229" t="s">
-        <v>166</v>
-      </c>
-      <c r="C229">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A230">
-        <v>229</v>
-      </c>
-      <c r="B230" t="s">
-        <v>167</v>
-      </c>
-      <c r="C230">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A231">
-        <v>230</v>
-      </c>
-      <c r="B231" t="s">
-        <v>168</v>
-      </c>
-      <c r="C231">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A232">
-        <v>231</v>
-      </c>
-      <c r="B232" t="s">
-        <v>169</v>
-      </c>
-      <c r="C232">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A233">
-        <v>232</v>
-      </c>
-      <c r="B233" t="s">
-        <v>170</v>
-      </c>
-      <c r="C233">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A234">
-        <v>233</v>
-      </c>
-      <c r="B234" t="s">
-        <v>171</v>
-      </c>
-      <c r="C234">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A235">
-        <v>234</v>
-      </c>
-      <c r="B235" t="s">
-        <v>172</v>
-      </c>
-      <c r="C235">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A236">
-        <v>235</v>
-      </c>
-      <c r="B236" t="s">
-        <v>173</v>
-      </c>
-      <c r="C236">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A237">
-        <v>236</v>
-      </c>
-      <c r="B237" t="s">
-        <v>174</v>
-      </c>
-      <c r="C237">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A238">
-        <v>237</v>
-      </c>
-      <c r="B238" t="s">
-        <v>175</v>
-      </c>
-      <c r="C238">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A239">
-        <v>238</v>
-      </c>
-      <c r="B239" t="s">
-        <v>176</v>
-      </c>
-      <c r="C239">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A240">
-        <v>239</v>
-      </c>
-      <c r="B240" t="s">
-        <v>148</v>
-      </c>
-      <c r="C240">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A241">
-        <v>240</v>
-      </c>
-      <c r="B241" t="s">
-        <v>149</v>
-      </c>
-      <c r="C241">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A242">
-        <v>241</v>
-      </c>
-      <c r="B242" t="s">
-        <v>150</v>
-      </c>
-      <c r="C242">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A243">
-        <v>242</v>
-      </c>
-      <c r="B243" t="s">
-        <v>151</v>
-      </c>
-      <c r="C243">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A244">
-        <v>243</v>
-      </c>
-      <c r="B244" t="s">
-        <v>161</v>
-      </c>
-      <c r="C244">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A245">
-        <v>244</v>
-      </c>
-      <c r="B245" t="s">
-        <v>162</v>
-      </c>
-      <c r="C245">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A246">
-        <v>245</v>
-      </c>
-      <c r="B246" t="s">
-        <v>163</v>
-      </c>
-      <c r="C246">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A247">
-        <v>246</v>
-      </c>
-      <c r="B247" t="s">
-        <v>164</v>
-      </c>
-      <c r="C247">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A248">
-        <v>247</v>
-      </c>
-      <c r="B248" t="s">
-        <v>165</v>
-      </c>
-      <c r="C248">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A249">
-        <v>248</v>
-      </c>
-      <c r="B249" t="s">
-        <v>166</v>
-      </c>
-      <c r="C249">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A250">
-        <v>249</v>
-      </c>
-      <c r="B250" t="s">
-        <v>167</v>
-      </c>
-      <c r="C250">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A251">
-        <v>250</v>
-      </c>
-      <c r="B251" t="s">
-        <v>168</v>
-      </c>
-      <c r="C251">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A252">
-        <v>251</v>
-      </c>
-      <c r="B252" t="s">
-        <v>169</v>
-      </c>
-      <c r="C252">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A253">
-        <v>252</v>
-      </c>
-      <c r="B253" t="s">
-        <v>170</v>
-      </c>
-      <c r="C253">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A254">
-        <v>253</v>
-      </c>
-      <c r="B254" t="s">
-        <v>171</v>
-      </c>
-      <c r="C254">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A255">
-        <v>254</v>
-      </c>
-      <c r="B255" t="s">
-        <v>172</v>
-      </c>
-      <c r="C255">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A256">
-        <v>255</v>
-      </c>
-      <c r="B256" t="s">
-        <v>173</v>
-      </c>
-      <c r="C256">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A257">
-        <v>256</v>
-      </c>
-      <c r="B257" t="s">
-        <v>174</v>
-      </c>
-      <c r="C257">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A258">
-        <v>257</v>
-      </c>
-      <c r="B258" t="s">
-        <v>175</v>
-      </c>
-      <c r="C258">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A259">
-        <v>258</v>
-      </c>
-      <c r="B259" t="s">
-        <v>176</v>
-      </c>
-      <c r="C259">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A260">
-        <v>259</v>
-      </c>
-      <c r="B260" t="s">
-        <v>148</v>
-      </c>
-      <c r="C260">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A261">
-        <v>260</v>
-      </c>
-      <c r="B261" t="s">
-        <v>149</v>
-      </c>
-      <c r="C261">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A262">
-        <v>261</v>
-      </c>
-      <c r="B262" t="s">
-        <v>150</v>
-      </c>
-      <c r="C262">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A263">
-        <v>262</v>
-      </c>
-      <c r="B263" t="s">
-        <v>151</v>
-      </c>
-      <c r="C263">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A264">
-        <v>263</v>
-      </c>
-      <c r="B264" t="s">
-        <v>161</v>
-      </c>
-      <c r="C264">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A265">
-        <v>264</v>
-      </c>
-      <c r="B265" t="s">
-        <v>162</v>
-      </c>
-      <c r="C265">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A266">
-        <v>265</v>
-      </c>
-      <c r="B266" t="s">
-        <v>163</v>
-      </c>
-      <c r="C266">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A267">
-        <v>266</v>
-      </c>
-      <c r="B267" t="s">
-        <v>164</v>
-      </c>
-      <c r="C267">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A268">
-        <v>267</v>
-      </c>
-      <c r="B268" t="s">
-        <v>165</v>
-      </c>
-      <c r="C268">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A269">
-        <v>268</v>
-      </c>
-      <c r="B269" t="s">
-        <v>166</v>
-      </c>
-      <c r="C269">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A270">
-        <v>269</v>
-      </c>
-      <c r="B270" t="s">
-        <v>167</v>
-      </c>
-      <c r="C270">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A271">
-        <v>270</v>
-      </c>
-      <c r="B271" t="s">
-        <v>168</v>
-      </c>
-      <c r="C271">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A272">
-        <v>271</v>
-      </c>
-      <c r="B272" t="s">
-        <v>169</v>
-      </c>
-      <c r="C272">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A273">
-        <v>272</v>
-      </c>
-      <c r="B273" t="s">
-        <v>170</v>
-      </c>
-      <c r="C273">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A274">
-        <v>273</v>
-      </c>
-      <c r="B274" t="s">
-        <v>171</v>
-      </c>
-      <c r="C274">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A275">
-        <v>274</v>
-      </c>
-      <c r="B275" t="s">
-        <v>172</v>
-      </c>
-      <c r="C275">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A276">
-        <v>275</v>
-      </c>
-      <c r="B276" t="s">
-        <v>173</v>
-      </c>
-      <c r="C276">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A277">
-        <v>276</v>
-      </c>
-      <c r="B277" t="s">
-        <v>174</v>
-      </c>
-      <c r="C277">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A278">
-        <v>277</v>
-      </c>
-      <c r="B278" t="s">
-        <v>175</v>
-      </c>
-      <c r="C278">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A279">
-        <v>278</v>
-      </c>
-      <c r="B279" t="s">
-        <v>176</v>
-      </c>
-      <c r="C279">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A280">
-        <v>279</v>
-      </c>
-      <c r="B280" t="s">
-        <v>148</v>
-      </c>
-      <c r="C280">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A281">
-        <v>280</v>
-      </c>
-      <c r="B281" t="s">
-        <v>149</v>
-      </c>
-      <c r="C281">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A282">
-        <v>281</v>
-      </c>
-      <c r="B282" t="s">
-        <v>150</v>
-      </c>
-      <c r="C282">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A283">
-        <v>282</v>
-      </c>
-      <c r="B283" t="s">
-        <v>151</v>
-      </c>
-      <c r="C283">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A284">
-        <v>283</v>
-      </c>
-      <c r="B284" t="s">
-        <v>161</v>
-      </c>
-      <c r="C284">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A285">
-        <v>284</v>
-      </c>
-      <c r="B285" t="s">
-        <v>162</v>
-      </c>
-      <c r="C285">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A286">
-        <v>285</v>
-      </c>
-      <c r="B286" t="s">
-        <v>163</v>
-      </c>
-      <c r="C286">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A287">
-        <v>286</v>
-      </c>
-      <c r="B287" t="s">
-        <v>164</v>
-      </c>
-      <c r="C287">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A288">
-        <v>287</v>
-      </c>
-      <c r="B288" t="s">
-        <v>165</v>
-      </c>
-      <c r="C288">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A289">
-        <v>288</v>
-      </c>
-      <c r="B289" t="s">
-        <v>166</v>
-      </c>
-      <c r="C289">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A290">
-        <v>289</v>
-      </c>
-      <c r="B290" t="s">
-        <v>167</v>
-      </c>
-      <c r="C290">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A291">
-        <v>290</v>
-      </c>
-      <c r="B291" t="s">
-        <v>168</v>
-      </c>
-      <c r="C291">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A292">
-        <v>291</v>
-      </c>
-      <c r="B292" t="s">
-        <v>169</v>
-      </c>
-      <c r="C292">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A293">
-        <v>292</v>
-      </c>
-      <c r="B293" t="s">
-        <v>170</v>
-      </c>
-      <c r="C293">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A294">
-        <v>293</v>
-      </c>
-      <c r="B294" t="s">
-        <v>171</v>
-      </c>
-      <c r="C294">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A295">
-        <v>294</v>
-      </c>
-      <c r="B295" t="s">
-        <v>172</v>
-      </c>
-      <c r="C295">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A296">
-        <v>295</v>
-      </c>
-      <c r="B296" t="s">
-        <v>173</v>
-      </c>
-      <c r="C296">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A297">
-        <v>296</v>
-      </c>
-      <c r="B297" t="s">
-        <v>174</v>
-      </c>
-      <c r="C297">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A298">
-        <v>297</v>
-      </c>
-      <c r="B298" t="s">
-        <v>175</v>
-      </c>
-      <c r="C298">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A299">
-        <v>298</v>
-      </c>
-      <c r="B299" t="s">
-        <v>176</v>
-      </c>
-      <c r="C299">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A300">
-        <v>299</v>
-      </c>
-      <c r="B300" t="s">
-        <v>148</v>
-      </c>
-      <c r="C300">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A301">
-        <v>300</v>
-      </c>
-      <c r="B301" t="s">
-        <v>149</v>
-      </c>
-      <c r="C301">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A302">
-        <v>301</v>
-      </c>
-      <c r="B302" t="s">
-        <v>150</v>
-      </c>
-      <c r="C302">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A303">
-        <v>302</v>
-      </c>
-      <c r="B303" t="s">
-        <v>151</v>
-      </c>
-      <c r="C303">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A304">
-        <v>303</v>
-      </c>
-      <c r="B304" t="s">
-        <v>161</v>
-      </c>
-      <c r="C304">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A305">
-        <v>304</v>
-      </c>
-      <c r="B305" t="s">
-        <v>162</v>
-      </c>
-      <c r="C305">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A306">
-        <v>305</v>
-      </c>
-      <c r="B306" t="s">
-        <v>163</v>
-      </c>
-      <c r="C306">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A307">
-        <v>306</v>
-      </c>
-      <c r="B307" t="s">
-        <v>164</v>
-      </c>
-      <c r="C307">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A308">
-        <v>307</v>
-      </c>
-      <c r="B308" t="s">
-        <v>165</v>
-      </c>
-      <c r="C308">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A309">
-        <v>308</v>
-      </c>
-      <c r="B309" t="s">
-        <v>166</v>
-      </c>
-      <c r="C309">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A310">
-        <v>309</v>
-      </c>
-      <c r="B310" t="s">
-        <v>167</v>
-      </c>
-      <c r="C310">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A311">
-        <v>310</v>
-      </c>
-      <c r="B311" t="s">
-        <v>168</v>
-      </c>
-      <c r="C311">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A312">
-        <v>311</v>
-      </c>
-      <c r="B312" t="s">
-        <v>169</v>
-      </c>
-      <c r="C312">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A313">
-        <v>312</v>
-      </c>
-      <c r="B313" t="s">
-        <v>170</v>
-      </c>
-      <c r="C313">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A314">
-        <v>313</v>
-      </c>
-      <c r="B314" t="s">
-        <v>171</v>
-      </c>
-      <c r="C314">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A315">
-        <v>314</v>
-      </c>
-      <c r="B315" t="s">
-        <v>172</v>
-      </c>
-      <c r="C315">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A316">
-        <v>315</v>
-      </c>
-      <c r="B316" t="s">
-        <v>173</v>
-      </c>
-      <c r="C316">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A317">
-        <v>316</v>
-      </c>
-      <c r="B317" t="s">
-        <v>174</v>
-      </c>
-      <c r="C317">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A318">
-        <v>317</v>
-      </c>
-      <c r="B318" t="s">
-        <v>175</v>
-      </c>
-      <c r="C318">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A319">
-        <v>318</v>
-      </c>
-      <c r="B319" t="s">
-        <v>176</v>
-      </c>
-      <c r="C319">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A320">
-        <v>319</v>
-      </c>
-      <c r="B320" t="s">
-        <v>148</v>
-      </c>
-      <c r="C320">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A321">
-        <v>320</v>
-      </c>
-      <c r="B321" t="s">
-        <v>149</v>
-      </c>
-      <c r="C321">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A322">
-        <v>321</v>
-      </c>
-      <c r="B322" t="s">
-        <v>150</v>
-      </c>
-      <c r="C322">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A323">
-        <v>322</v>
-      </c>
-      <c r="B323" t="s">
-        <v>151</v>
-      </c>
-      <c r="C323">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A324">
-        <v>323</v>
-      </c>
-      <c r="B324" t="s">
-        <v>161</v>
-      </c>
-      <c r="C324">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A325">
-        <v>324</v>
-      </c>
-      <c r="B325" t="s">
-        <v>162</v>
-      </c>
-      <c r="C325">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pills replaced with search box for categories
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4D21A9-0A6D-4558-BE6D-6D7C92FD6671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BBBD6D-697E-4D98-AC4F-408381C417DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548F3BD-78D7-4C41-AEEB-86055749FC7F}">
   <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,7 +1025,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5">
@@ -1036,7 +1036,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6">

</xml_diff>

<commit_message>
my account details added
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF05A15F-160A-453D-A07D-FA59676E42D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775D8D51-285A-45B6-B708-4E09C348C785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548F3BD-78D7-4C41-AEEB-86055749FC7F}">
   <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,7 +1135,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15">

</xml_diff>

<commit_message>
send email button added
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B463106-45C2-460A-B01E-A376565628A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884865C7-C3C0-40F7-985E-562BC8FF5EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -969,7 +969,7 @@
   <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1190,7 +1190,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C20">

</xml_diff>